<commit_message>
Updated an error message
</commit_message>
<xml_diff>
--- a/docs/requirements/Requirements Detailing References/ID-Authentication/Sprint 11/Consolidated error messages V2.4.xlsx
+++ b/docs/requirements/Requirements Detailing References/ID-Authentication/Sprint 11/Consolidated error messages V2.4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIPRequirementsGithub\docs\requirements\Requirements Detailing References\ID-Authentication\Sprint 11\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{207CEA37-01E4-4EE0-B805-6CA5400FE3B2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{52C09C66-0368-45C2-80B6-EF89CE93A458}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1164,13 +1164,13 @@
     <t>"Could not revoke VID"</t>
   </si>
   <si>
-    <t>Could not generate VID as the max no of instances is reached</t>
-  </si>
-  <si>
-    <t>"Could not generate/regenerate VID - max no of instances has been generated"</t>
-  </si>
-  <si>
     <t>IDA-MLC-021</t>
+  </si>
+  <si>
+    <t>Could not generate VID as the max no of instances is reached/manual regeneration not allowed as per policy</t>
+  </si>
+  <si>
+    <t>"Could not generate/regenerate VID as per policy"</t>
   </si>
 </sst>
 </file>
@@ -1393,7 +1393,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1454,6 +1454,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1802,8 +1805,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:L70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="J70" sqref="J70"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.7109375" defaultRowHeight="28.5" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -2099,7 +2102,7 @@
       </c>
       <c r="G14" s="8"/>
     </row>
-    <row r="15" spans="1:12" ht="63" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" ht="78.75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -2141,7 +2144,7 @@
       </c>
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="1:7" ht="31.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="47.25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -2160,7 +2163,7 @@
       </c>
       <c r="G17" s="8"/>
     </row>
-    <row r="18" spans="1:7" ht="78.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="94.5" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -3056,7 +3059,7 @@
       <c r="G67" s="6"/>
     </row>
     <row r="68" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="4">
+      <c r="A68" s="26">
         <v>70</v>
       </c>
       <c r="B68" s="18" t="s">
@@ -3088,27 +3091,23 @@
         <v>303</v>
       </c>
       <c r="G69" s="18"/>
-      <c r="H69" s="6"/>
-      <c r="I69" s="6"/>
-      <c r="J69" s="6"/>
-    </row>
-    <row r="70" spans="1:11" ht="47.25" x14ac:dyDescent="0.2">
-      <c r="A70" s="12">
+    </row>
+    <row r="70" spans="1:11" ht="78.75" x14ac:dyDescent="0.2">
+      <c r="A70" s="18">
         <v>72</v>
       </c>
       <c r="B70" s="18" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C70" s="18" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D70" s="18"/>
       <c r="E70" s="18"/>
       <c r="F70" s="18" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="G70" s="18"/>
-      <c r="J70" s="18"/>
       <c r="K70" s="18"/>
     </row>
   </sheetData>

</xml_diff>